<commit_message>
changed ID back to original one
</commit_message>
<xml_diff>
--- a/templates/dataplant/MIMS_minimal-Metagenomics.xlsx
+++ b/templates/dataplant/MIMS_minimal-Metagenomics.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stella Eggels\sciebo - Eggels, Stella (s.eggels@fz-juelich.de)@fz-juelich.sciebo.de\SE\DataPLANT\Metadata completeness u swate templates meetings\SWATE templates meetings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stella Eggels\Documents\GitHub\Swate-templates\templates\dataplant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD0C1EF-B757-439D-8087-D1230F6A426B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE05C02-739A-41B3-9FD5-28BFB7A89ABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{FFC9D3F5-1023-433E-A50A-7D9CDA7F418D}"/>
   </bookViews>
@@ -351,9 +351,6 @@
     <t>Template term</t>
   </si>
   <si>
-    <t>96bb7d4a-74b0-4558-a5c8-8595ca64bf93</t>
-  </si>
-  <si>
     <t>Characteristic [GPS coordinates]</t>
   </si>
   <si>
@@ -361,6 +358,9 @@
   </si>
   <si>
     <t>Term Accession Number (AGRO:00000572)</t>
+  </si>
+  <si>
+    <t>b0d579bd-8045-4b1c-b836-5c46ec19af2b</t>
   </si>
 </sst>
 </file>
@@ -669,12 +669,12 @@
     <tableColumn id="24" xr3:uid="{AA8FB106-A079-4FCB-84DB-C4B192C0458B}" name="Characteristic [geographic location]" dataDxfId="8"/>
     <tableColumn id="25" xr3:uid="{FE8330FC-7175-4199-BA23-11B1720DF94F}" name="Term Source REF (GAZ:00000448)" dataDxfId="7"/>
     <tableColumn id="26" xr3:uid="{1D106C0A-5BA8-4541-9BF4-8AECD8A98EAA}" name="Term Accession Number (GAZ:00000448)" dataDxfId="6"/>
-    <tableColumn id="1" xr3:uid="{E8AB71EC-F841-4A49-827E-F93FC14DA3A5}" name="Characteristic [GPS coordinates]" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{78AA52D5-8314-482A-A6D3-3EB4CBCBA400}" name="Term Source REF (AGRO:00000572)" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{1D39C1C4-E81C-49E0-B5AB-DC1D2EEA6115}" name="Term Accession Number (AGRO:00000572)" dataDxfId="0"/>
-    <tableColumn id="41" xr3:uid="{F7839284-E793-418E-85BC-804F6C8C08BF}" name="Parameter [sequencing method]" dataDxfId="5"/>
-    <tableColumn id="42" xr3:uid="{E95A192F-E6D5-4A81-AB7B-AFEF38154231}" name="Term Source REF (DPBO:0002006)" dataDxfId="4"/>
-    <tableColumn id="43" xr3:uid="{4AD9FAAC-75CE-48AA-930C-733ADD252CF4}" name="Term Accession Number (DPBO:0002006)" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{E8AB71EC-F841-4A49-827E-F93FC14DA3A5}" name="Characteristic [GPS coordinates]" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{78AA52D5-8314-482A-A6D3-3EB4CBCBA400}" name="Term Source REF (AGRO:00000572)" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{1D39C1C4-E81C-49E0-B5AB-DC1D2EEA6115}" name="Term Accession Number (AGRO:00000572)" dataDxfId="3"/>
+    <tableColumn id="41" xr3:uid="{F7839284-E793-418E-85BC-804F6C8C08BF}" name="Parameter [sequencing method]" dataDxfId="2"/>
+    <tableColumn id="42" xr3:uid="{E95A192F-E6D5-4A81-AB7B-AFEF38154231}" name="Term Source REF (DPBO:0002006)" dataDxfId="1"/>
+    <tableColumn id="43" xr3:uid="{4AD9FAAC-75CE-48AA-930C-733ADD252CF4}" name="Term Accession Number (DPBO:0002006)" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{74FB988B-0DE5-4CAD-8A88-EC046C59C7D1}" name="Sample Name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1134,13 +1134,13 @@
         <v>14</v>
       </c>
       <c r="T1" t="s">
+        <v>73</v>
+      </c>
+      <c r="U1" t="s">
         <v>74</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>75</v>
-      </c>
-      <c r="V1" t="s">
-        <v>76</v>
       </c>
       <c r="W1" t="s">
         <v>51</v>
@@ -1246,7 +1246,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1260,7 +1260,7 @@
         <v>15</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1529,7 +1529,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B10" t="s">
         <v>67</v>

</xml_diff>